<commit_message>
now i will use server
</commit_message>
<xml_diff>
--- a/documents/other/change_rate_representative.xlsx
+++ b/documents/other/change_rate_representative.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,9 @@
       <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -456,6 +459,9 @@
       </c>
       <c r="D2" t="n">
         <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.001884944920440637</v>
       </c>
     </row>
     <row r="3">
@@ -471,6 +477,9 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.002281926303347229</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -485,6 +494,9 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
+      <c r="E4" t="n">
+        <v>-0.0004456408577852223</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -499,6 +511,9 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.002325581395348837</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -513,6 +528,9 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.002308815810710199</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -527,6 +545,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.002316777923169888</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -541,6 +562,9 @@
       <c r="D8" t="n">
         <v>-0.05501179541233747</v>
       </c>
+      <c r="E8" t="n">
+        <v>-0.001942167266456478</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -555,6 +579,9 @@
       <c r="D9" t="n">
         <v>-0.1864074954551811</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.0008844103768215862</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -569,6 +596,9 @@
       <c r="D10" t="n">
         <v>-0.06476521928274293</v>
       </c>
+      <c r="E10" t="n">
+        <v>-0.001206072474370804</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -583,6 +613,9 @@
       <c r="D11" t="n">
         <v>0.02704207428616878</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.001031927034490668</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -597,6 +630,9 @@
       <c r="D12" t="n">
         <v>0</v>
       </c>
+      <c r="E12" t="n">
+        <v>2.214839424141677e-05</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -611,6 +647,9 @@
       <c r="D13" t="n">
         <v>-0.04511278195488722</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.0002972547648190249</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -625,6 +664,9 @@
       <c r="D14" t="n">
         <v>0</v>
       </c>
+      <c r="E14" t="n">
+        <v>-2.768549280177161e-05</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -639,6 +681,9 @@
       <c r="D15" t="n">
         <v>0</v>
       </c>
+      <c r="E15" t="n">
+        <v>-0.0004228329809725159</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -653,6 +698,9 @@
       <c r="D16" t="n">
         <v>0</v>
       </c>
+      <c r="E16" t="n">
+        <v>-0.000225616105518917</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -667,6 +715,9 @@
       <c r="D17" t="n">
         <v>0</v>
       </c>
+      <c r="E17" t="n">
+        <v>-0.0002474022761009403</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -681,6 +732,9 @@
       <c r="D18" t="n">
         <v>0</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.002325581395348837</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -695,6 +749,9 @@
       <c r="D19" t="n">
         <v>0</v>
       </c>
+      <c r="E19" t="n">
+        <v>-0.001223990208078335</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -709,6 +766,9 @@
       <c r="D20" t="n">
         <v>-0.00317234484349771</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.0006536505886834703</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -723,6 +783,9 @@
       <c r="D21" t="n">
         <v>-0.001697530864197522</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.0008347688774045363</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -736,6 +799,9 @@
       </c>
       <c r="D22" t="n">
         <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.002325581395348837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>